<commit_message>
Add `task-13` in `econometrics`
</commit_message>
<xml_diff>
--- a/3-course-6-semester/econometrics/task-11/task-11.xlsx
+++ b/3-course-6-semester/econometrics/task-11/task-11.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mag\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bronn\Documents\github\university\3-course-6-semester\econometrics\task-11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECB2436-D3ED-4F55-BB65-3DE18E6B332D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F81280-EF3F-47B0-80B8-089654CBB974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="4560" windowWidth="20730" windowHeight="11310" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ДЗ №1" sheetId="1" r:id="rId1"/>
@@ -28,10 +28,20 @@
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="179021" iterate="1" iterateCount="1" iterateDelta="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -995,9 +1005,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1019,12 +1026,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1079,13 +1080,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1181,7 +1191,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ru-RU"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1263,7 +1273,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="ru-RU"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1313,7 +1323,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="ru-RU"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1364,7 +1374,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="ru-RU"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1414,7 +1424,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="ru-RU"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1465,7 +1475,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="ru-RU"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1557,7 +1567,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1565144240"/>
@@ -1616,7 +1626,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1565142160"/>
@@ -1664,7 +1674,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="ru-RU"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1837,7 +1847,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="95811344"/>
@@ -1899,7 +1909,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="95808064"/>
@@ -1947,7 +1957,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="ru-RU"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4799,7 +4809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B5:D12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
@@ -4863,7 +4873,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471091B4-CFBF-41FA-8B21-FF23AFEAB06C}">
   <dimension ref="A3:AE72"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M70" sqref="M70"/>
     </sheetView>
   </sheetViews>
@@ -4891,16 +4901,16 @@
       <c r="E4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="42" t="s">
+      <c r="F4" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="42" t="s">
+      <c r="G4" s="41" t="s">
         <v>48</v>
       </c>
       <c r="H4" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="I4" s="41" t="s">
+      <c r="I4" s="40" t="s">
         <v>50</v>
       </c>
     </row>
@@ -4919,14 +4929,14 @@
       <c r="E5" s="12">
         <v>2</v>
       </c>
-      <c r="F5" s="43">
+      <c r="F5" s="42">
         <f>($B$12-B5)^2</f>
         <v>6.25</v>
       </c>
-      <c r="G5" s="47" t="s">
+      <c r="G5" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="51" t="s">
+      <c r="H5" s="50" t="s">
         <v>47</v>
       </c>
       <c r="I5">
@@ -4949,15 +4959,15 @@
       <c r="E6" s="4">
         <v>4</v>
       </c>
-      <c r="F6" s="43">
+      <c r="F6" s="42">
         <f>($B$12-B6)^2</f>
         <v>2.25</v>
       </c>
-      <c r="G6" s="48">
+      <c r="G6" s="47">
         <f>E6/E5</f>
         <v>2</v>
       </c>
-      <c r="H6" s="50" t="s">
+      <c r="H6" s="49" t="s">
         <v>47</v>
       </c>
       <c r="I6">
@@ -4980,15 +4990,15 @@
       <c r="E7" s="4">
         <v>10</v>
       </c>
-      <c r="F7" s="43">
+      <c r="F7" s="42">
         <f>(B15-B7)^2</f>
         <v>9</v>
       </c>
-      <c r="G7" s="48">
+      <c r="G7" s="47">
         <f t="shared" ref="G7:G10" si="3">E7/E6</f>
         <v>2.5</v>
       </c>
-      <c r="H7" s="45">
+      <c r="H7" s="44">
         <f>G7/G6</f>
         <v>1.25</v>
       </c>
@@ -5012,15 +5022,15 @@
       <c r="E8" s="4">
         <v>31</v>
       </c>
-      <c r="F8" s="43">
+      <c r="F8" s="42">
         <f>(B16-B8)^2</f>
         <v>16</v>
       </c>
-      <c r="G8" s="48">
+      <c r="G8" s="47">
         <f t="shared" si="3"/>
         <v>3.1</v>
       </c>
-      <c r="H8" s="45">
+      <c r="H8" s="44">
         <f t="shared" ref="H8:H10" si="4">G8/G7</f>
         <v>1.24</v>
       </c>
@@ -5044,15 +5054,15 @@
       <c r="E9" s="4">
         <v>117</v>
       </c>
-      <c r="F9" s="43">
+      <c r="F9" s="42">
         <f>(B17-B9)^2</f>
         <v>25</v>
       </c>
-      <c r="G9" s="48">
+      <c r="G9" s="47">
         <f t="shared" si="3"/>
         <v>3.774193548387097</v>
       </c>
-      <c r="H9" s="45">
+      <c r="H9" s="44">
         <f t="shared" si="4"/>
         <v>1.2174817898022894</v>
       </c>
@@ -5076,15 +5086,15 @@
       <c r="E10" s="4">
         <v>550</v>
       </c>
-      <c r="F10" s="43">
+      <c r="F10" s="42">
         <f>(B18-B10)^2</f>
         <v>36</v>
       </c>
-      <c r="G10" s="49">
+      <c r="G10" s="48">
         <f t="shared" si="3"/>
         <v>4.700854700854701</v>
       </c>
-      <c r="H10" s="46">
+      <c r="H10" s="45">
         <f t="shared" si="4"/>
         <v>1.2455256044999634</v>
       </c>
@@ -5130,10 +5140,10 @@
         <v>7</v>
       </c>
       <c r="C21" s="20"/>
-      <c r="N21" s="40" t="s">
+      <c r="N21" s="85" t="s">
         <v>33</v>
       </c>
-      <c r="O21" s="40"/>
+      <c r="O21" s="85"/>
     </row>
     <row r="22" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="17" t="s">
@@ -5145,7 +5155,7 @@
       <c r="N22" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="O22" s="55">
+      <c r="O22" s="52">
         <f>Q45*Q46^7*Q47^49</f>
         <v>3194.1265275704677</v>
       </c>
@@ -5310,10 +5320,10 @@
       <c r="T33" s="17">
         <v>0.99999671963775649</v>
       </c>
-      <c r="AD33" s="53" t="s">
+      <c r="AD33" s="86" t="s">
         <v>33</v>
       </c>
-      <c r="AE33" s="54"/>
+      <c r="AE33" s="87"/>
     </row>
     <row r="34" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="19"/>
@@ -5602,7 +5612,7 @@
       <c r="D45" s="17">
         <v>47.32142857142864</v>
       </c>
-      <c r="P45" s="52" t="s">
+      <c r="P45" s="51" t="s">
         <v>52</v>
       </c>
       <c r="Q45">
@@ -5647,7 +5657,7 @@
       <c r="D46" s="17">
         <v>53.142857142857167</v>
       </c>
-      <c r="P46" s="52" t="s">
+      <c r="P46" s="51" t="s">
         <v>53</v>
       </c>
       <c r="Q46">
@@ -5692,7 +5702,7 @@
       <c r="D47" s="17">
         <v>-14.428571428571445</v>
       </c>
-      <c r="P47" s="52" t="s">
+      <c r="P47" s="51" t="s">
         <v>54</v>
       </c>
       <c r="Q47">
@@ -5790,7 +5800,7 @@
       </c>
     </row>
     <row r="55" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I55" s="56" t="s">
+      <c r="I55" s="53" t="s">
         <v>1</v>
       </c>
       <c r="J55">
@@ -5814,10 +5824,10 @@
       <c r="D56" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F56" s="40" t="s">
+      <c r="F56" s="85" t="s">
         <v>33</v>
       </c>
-      <c r="G56" s="40"/>
+      <c r="G56" s="85"/>
       <c r="S56" s="17">
         <v>3</v>
       </c>
@@ -6126,7 +6136,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA2CED6-8A77-4828-832C-ED6E61706C02}">
   <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
@@ -6137,33 +6147,33 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="64" t="s">
+      <c r="D2" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="64" t="s">
+      <c r="E2" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="65" t="s">
+      <c r="F2" s="62" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="72">
+      <c r="B3" s="69">
         <v>1</v>
       </c>
-      <c r="C3" s="78">
+      <c r="C3" s="75">
         <v>12</v>
       </c>
-      <c r="D3" s="72">
+      <c r="D3" s="69">
         <v>0</v>
       </c>
-      <c r="E3" s="69">
+      <c r="E3" s="66">
         <f>COS(D3)</f>
         <v>1</v>
       </c>
@@ -6173,17 +6183,17 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="45">
+      <c r="B4" s="44">
         <v>2</v>
       </c>
-      <c r="C4" s="79">
+      <c r="C4" s="76">
         <v>11</v>
       </c>
-      <c r="D4" s="45">
+      <c r="D4" s="44">
         <f>2*PI()/$B$14</f>
         <v>0.52359877559829882</v>
       </c>
-      <c r="E4" s="70">
+      <c r="E4" s="67">
         <f t="shared" ref="E4:E14" si="0">COS(D4)</f>
         <v>0.86602540378443871</v>
       </c>
@@ -6193,17 +6203,17 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="45">
+      <c r="B5" s="44">
         <v>3</v>
       </c>
-      <c r="C5" s="79">
+      <c r="C5" s="76">
         <v>10</v>
       </c>
-      <c r="D5" s="45">
+      <c r="D5" s="44">
         <f>D4+$D$4</f>
         <v>1.0471975511965976</v>
       </c>
-      <c r="E5" s="70">
+      <c r="E5" s="67">
         <f t="shared" si="0"/>
         <v>0.50000000000000011</v>
       </c>
@@ -6213,17 +6223,17 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="45">
+      <c r="B6" s="44">
         <v>4</v>
       </c>
-      <c r="C6" s="79">
+      <c r="C6" s="76">
         <v>10</v>
       </c>
-      <c r="D6" s="45">
+      <c r="D6" s="44">
         <f t="shared" ref="D6:D16" si="2">D5+$D$4</f>
         <v>1.5707963267948966</v>
       </c>
-      <c r="E6" s="70">
+      <c r="E6" s="67">
         <f t="shared" si="0"/>
         <v>6.1257422745431001E-17</v>
       </c>
@@ -6233,17 +6243,17 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="45">
+      <c r="B7" s="44">
         <v>5</v>
       </c>
-      <c r="C7" s="79">
+      <c r="C7" s="76">
         <v>11</v>
       </c>
-      <c r="D7" s="45">
+      <c r="D7" s="44">
         <f t="shared" si="2"/>
         <v>2.0943951023931953</v>
       </c>
-      <c r="E7" s="70">
+      <c r="E7" s="67">
         <f t="shared" si="0"/>
         <v>-0.49999999999999978</v>
       </c>
@@ -6253,17 +6263,17 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="45">
+      <c r="B8" s="44">
         <v>6</v>
       </c>
-      <c r="C8" s="79">
+      <c r="C8" s="76">
         <v>12</v>
       </c>
-      <c r="D8" s="45">
+      <c r="D8" s="44">
         <f t="shared" si="2"/>
         <v>2.617993877991494</v>
       </c>
-      <c r="E8" s="70">
+      <c r="E8" s="67">
         <f t="shared" si="0"/>
         <v>-0.86602540378443849</v>
       </c>
@@ -6273,17 +6283,17 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="45">
+      <c r="B9" s="44">
         <v>7</v>
       </c>
-      <c r="C9" s="79">
+      <c r="C9" s="76">
         <v>12</v>
       </c>
-      <c r="D9" s="45">
+      <c r="D9" s="44">
         <f t="shared" si="2"/>
         <v>3.1415926535897927</v>
       </c>
-      <c r="E9" s="70">
+      <c r="E9" s="67">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
@@ -6293,17 +6303,17 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="45">
+      <c r="B10" s="44">
         <v>8</v>
       </c>
-      <c r="C10" s="79">
+      <c r="C10" s="76">
         <v>14</v>
       </c>
-      <c r="D10" s="45">
+      <c r="D10" s="44">
         <f t="shared" si="2"/>
         <v>3.6651914291880914</v>
       </c>
-      <c r="E10" s="70">
+      <c r="E10" s="67">
         <f t="shared" si="0"/>
         <v>-0.86602540378443904</v>
       </c>
@@ -6313,17 +6323,17 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="45">
+      <c r="B11" s="44">
         <v>9</v>
       </c>
-      <c r="C11" s="79">
+      <c r="C11" s="76">
         <v>14</v>
       </c>
-      <c r="D11" s="45">
+      <c r="D11" s="44">
         <f t="shared" si="2"/>
         <v>4.1887902047863905</v>
       </c>
-      <c r="E11" s="70">
+      <c r="E11" s="67">
         <f t="shared" si="0"/>
         <v>-0.50000000000000044</v>
       </c>
@@ -6333,17 +6343,17 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="45">
+      <c r="B12" s="44">
         <v>10</v>
       </c>
-      <c r="C12" s="79">
+      <c r="C12" s="76">
         <v>13</v>
       </c>
-      <c r="D12" s="45">
+      <c r="D12" s="44">
         <f t="shared" si="2"/>
         <v>4.7123889803846897</v>
       </c>
-      <c r="E12" s="70">
+      <c r="E12" s="67">
         <f t="shared" si="0"/>
         <v>-1.83772268236293E-16</v>
       </c>
@@ -6353,17 +6363,17 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="45">
+      <c r="B13" s="44">
         <v>11</v>
       </c>
-      <c r="C13" s="79">
+      <c r="C13" s="76">
         <v>12</v>
       </c>
-      <c r="D13" s="45">
+      <c r="D13" s="44">
         <f t="shared" si="2"/>
         <v>5.2359877559829888</v>
       </c>
-      <c r="E13" s="70">
+      <c r="E13" s="67">
         <f t="shared" si="0"/>
         <v>0.50000000000000011</v>
       </c>
@@ -6373,17 +6383,17 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="73">
+      <c r="B14" s="70">
         <v>12</v>
       </c>
-      <c r="C14" s="80">
+      <c r="C14" s="77">
         <v>11</v>
       </c>
-      <c r="D14" s="73">
+      <c r="D14" s="70">
         <f t="shared" si="2"/>
         <v>5.759586531581288</v>
       </c>
-      <c r="E14" s="71">
+      <c r="E14" s="68">
         <f t="shared" si="0"/>
         <v>0.86602540378443882</v>
       </c>
@@ -6393,52 +6403,52 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="68" t="s">
+      <c r="A15" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="74">
+      <c r="B15" s="71">
         <v>13</v>
       </c>
-      <c r="C15" s="76">
+      <c r="C15" s="73">
         <f>SUM(C3:C14)</f>
         <v>142</v>
       </c>
-      <c r="D15" s="45">
+      <c r="D15" s="44">
         <f t="shared" si="2"/>
         <v>6.2831853071795871</v>
       </c>
-      <c r="E15" s="77">
+      <c r="E15" s="74">
         <f>SUM(E3:E14)</f>
         <v>0</v>
       </c>
-      <c r="F15" s="67">
+      <c r="F15" s="64">
         <f>SUM(F3:F14)</f>
         <v>1.8873791418627661E-15</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="75">
+      <c r="B16" s="72">
         <v>14</v>
       </c>
-      <c r="D16" s="46">
+      <c r="D16" s="45">
         <f t="shared" si="2"/>
         <v>6.8067840827778863</v>
       </c>
-      <c r="E16" s="81">
+      <c r="E16" s="78">
         <f>COS(D16)</f>
         <v>0.86602540378443815</v>
       </c>
-      <c r="F16" s="66">
+      <c r="F16" s="63">
         <f>SIN(D16)</f>
         <v>0.50000000000000078</v>
       </c>
     </row>
     <row r="18" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="62" t="s">
+      <c r="B19" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="61">
+      <c r="C19" s="58">
         <f>AVERAGE(C3:C14)</f>
         <v>11.833333333333334</v>
       </c>
@@ -6447,7 +6457,7 @@
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="L20" s="82">
+      <c r="L20" s="79">
         <f>C37+C38*E16+C39*F16</f>
         <v>10.422649730810374</v>
       </c>
@@ -6863,180 +6873,180 @@
   <sheetData>
     <row r="5" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="85" t="s">
+      <c r="C6" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="86" t="s">
+      <c r="D6" s="83" t="s">
         <v>62</v>
       </c>
-      <c r="E6" s="86" t="s">
+      <c r="E6" s="83" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="86" t="s">
+      <c r="F6" s="83" t="s">
         <v>64</v>
       </c>
-      <c r="G6" s="86" t="s">
+      <c r="G6" s="83" t="s">
         <v>66</v>
       </c>
-      <c r="H6" s="87" t="s">
+      <c r="H6" s="84" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="83">
+      <c r="C7" s="80">
         <v>1</v>
       </c>
-      <c r="D7" s="84">
+      <c r="D7" s="81">
         <v>0</v>
       </c>
-      <c r="E7" s="89" t="s">
+      <c r="E7" s="88" t="s">
         <v>68</v>
       </c>
-      <c r="F7" s="89"/>
-      <c r="G7" s="89"/>
-      <c r="H7" s="90"/>
+      <c r="F7" s="88"/>
+      <c r="G7" s="88"/>
+      <c r="H7" s="89"/>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C8" s="3">
         <v>2</v>
       </c>
-      <c r="D8" s="44">
+      <c r="D8" s="43">
         <f>2*PI()/C16</f>
         <v>0.62831853071795862</v>
       </c>
-      <c r="E8" s="88"/>
-      <c r="F8" s="88"/>
-      <c r="G8" s="88"/>
+      <c r="E8" s="90"/>
+      <c r="F8" s="90"/>
+      <c r="G8" s="90"/>
       <c r="H8" s="91"/>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C9" s="3">
         <v>3</v>
       </c>
-      <c r="D9" s="44">
+      <c r="D9" s="43">
         <f>D8+$D$8</f>
         <v>1.2566370614359172</v>
       </c>
-      <c r="E9" s="88"/>
-      <c r="F9" s="88"/>
-      <c r="G9" s="88"/>
+      <c r="E9" s="90"/>
+      <c r="F9" s="90"/>
+      <c r="G9" s="90"/>
       <c r="H9" s="91"/>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C10" s="3">
         <v>4</v>
       </c>
-      <c r="D10" s="44">
+      <c r="D10" s="43">
         <f t="shared" ref="D10:D17" si="0">D9+$D$8</f>
         <v>1.8849555921538759</v>
       </c>
-      <c r="E10" s="88"/>
-      <c r="F10" s="88"/>
-      <c r="G10" s="88"/>
+      <c r="E10" s="90"/>
+      <c r="F10" s="90"/>
+      <c r="G10" s="90"/>
       <c r="H10" s="91"/>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C11" s="3">
         <v>5</v>
       </c>
-      <c r="D11" s="44">
+      <c r="D11" s="43">
         <f t="shared" si="0"/>
         <v>2.5132741228718345</v>
       </c>
-      <c r="E11" s="88"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="88"/>
+      <c r="E11" s="90"/>
+      <c r="F11" s="90"/>
+      <c r="G11" s="90"/>
       <c r="H11" s="91"/>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C12" s="3">
         <v>6</v>
       </c>
-      <c r="D12" s="44">
+      <c r="D12" s="43">
         <f t="shared" si="0"/>
         <v>3.1415926535897931</v>
       </c>
-      <c r="E12" s="88"/>
-      <c r="F12" s="88"/>
-      <c r="G12" s="88"/>
+      <c r="E12" s="90"/>
+      <c r="F12" s="90"/>
+      <c r="G12" s="90"/>
       <c r="H12" s="91"/>
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C13" s="3">
         <v>7</v>
       </c>
-      <c r="D13" s="44">
+      <c r="D13" s="43">
         <f t="shared" si="0"/>
         <v>3.7699111843077517</v>
       </c>
-      <c r="E13" s="88"/>
-      <c r="F13" s="88"/>
-      <c r="G13" s="88"/>
+      <c r="E13" s="90"/>
+      <c r="F13" s="90"/>
+      <c r="G13" s="90"/>
       <c r="H13" s="91"/>
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C14" s="3">
         <v>8</v>
       </c>
-      <c r="D14" s="44">
+      <c r="D14" s="43">
         <f t="shared" si="0"/>
         <v>4.3982297150257104</v>
       </c>
-      <c r="E14" s="88"/>
-      <c r="F14" s="88"/>
-      <c r="G14" s="88"/>
+      <c r="E14" s="90"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="90"/>
       <c r="H14" s="91"/>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C15" s="3">
         <v>9</v>
       </c>
-      <c r="D15" s="44">
+      <c r="D15" s="43">
         <f t="shared" si="0"/>
         <v>5.026548245743669</v>
       </c>
-      <c r="E15" s="88"/>
-      <c r="F15" s="88"/>
-      <c r="G15" s="88"/>
+      <c r="E15" s="90"/>
+      <c r="F15" s="90"/>
+      <c r="G15" s="90"/>
       <c r="H15" s="91"/>
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C16" s="3">
         <v>10</v>
       </c>
-      <c r="D16" s="44">
+      <c r="D16" s="43">
         <f t="shared" si="0"/>
         <v>5.6548667764616276</v>
       </c>
-      <c r="E16" s="88"/>
-      <c r="F16" s="88"/>
-      <c r="G16" s="88"/>
+      <c r="E16" s="90"/>
+      <c r="F16" s="90"/>
+      <c r="G16" s="90"/>
       <c r="H16" s="91"/>
     </row>
     <row r="17" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="58">
+      <c r="C17" s="55">
         <v>11</v>
       </c>
-      <c r="D17" s="59">
+      <c r="D17" s="56">
         <f t="shared" si="0"/>
         <v>6.2831853071795862</v>
       </c>
-      <c r="E17" s="59">
+      <c r="E17" s="56">
         <f>COS(D17)</f>
         <v>1</v>
       </c>
-      <c r="F17" s="59">
+      <c r="F17" s="56">
         <v>0</v>
       </c>
-      <c r="G17" s="59">
+      <c r="G17" s="56">
         <v>1</v>
       </c>
-      <c r="H17" s="60">
+      <c r="H17" s="57">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="E20" s="56" t="s">
+      <c r="E20" s="53" t="s">
         <v>32</v>
       </c>
       <c r="F20">
@@ -7045,7 +7055,7 @@
       </c>
     </row>
     <row r="25" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="D25" s="57" t="s">
+      <c r="D25" s="54" t="s">
         <v>69</v>
       </c>
     </row>
@@ -7056,10 +7066,10 @@
       </c>
     </row>
     <row r="28" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="G28" s="57" t="s">
+      <c r="G28" s="54" t="s">
         <v>70</v>
       </c>
-      <c r="K28" s="57" t="s">
+      <c r="K28" s="54" t="s">
         <v>33</v>
       </c>
     </row>
@@ -7083,7 +7093,7 @@
       <c r="C30">
         <v>1</v>
       </c>
-      <c r="D30" s="84">
+      <c r="D30" s="81">
         <v>0</v>
       </c>
     </row>
@@ -7280,8 +7290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAAF0091-F4C3-4F65-8C34-C6C7EC533D71}">
   <dimension ref="C3:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>